<commit_message>
.vue and interface for implements are generatable now. * generate typescript class for component.
</commit_message>
<xml_diff>
--- a/meta/components/TableSample.xlsx
+++ b/meta/components/TableSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD9498C-3554-304F-8A97-1D24B9C000D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B50B1B-1803-E849-8D05-AC36CF7C7A84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="1240" windowWidth="25200" windowHeight="19620" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13200" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
-  <si>
-    <t>クラス名</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
   <si>
     <t>パッケージ</t>
   </si>
@@ -87,10 +84,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>パッケージ</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>様式 ver 0.0.2 (2019.01.23)</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -223,10 +216,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>oplux.v3.views.tableSample</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>種別</t>
     <rPh sb="0" eb="2">
       <t xml:space="preserve">シュベツ </t>
@@ -306,10 +295,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Vueコンポーネント定義・継承</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Vueコンポーネント定義・ヘッダ情報</t>
     <rPh sb="0" eb="18">
       <t xml:space="preserve">ジョウホウ </t>
@@ -333,22 +318,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>/* Vue クラス以外を継承する場合はここに指定します */</t>
-    <rPh sb="10" eb="12">
-      <t xml:space="preserve">イガイ </t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t xml:space="preserve">ケイショウ </t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t xml:space="preserve">バアイハ </t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t xml:space="preserve">シテイ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Vueコンポーネント定義・プロパティ</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -455,10 +424,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>@/components</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>/table</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -526,6 +491,102 @@
       <t xml:space="preserve">シヨウ </t>
     </rPh>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>sample.views.tableSample</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@/views/tableSample</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prop01</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>""</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prop02</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>二つ目のプロパティです</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">フタツメノ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prop03</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>array</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ObjectSample</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>三つ目のプロパティです</t>
+    <rPh sb="0" eb="1">
+      <t>ミッツメ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>一つ目のプロパティです</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ヒトツメノ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>コンポーネントID</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>テーブルサンプル</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* 変数定義されます, i18n などと併用する場合は、ここにタグを記述します */</t>
+    <rPh sb="3" eb="7">
+      <t xml:space="preserve">ヘンスウテイギ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">ヘイヨウスル </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prop04</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>四つ目のプロパティです</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">４ツメ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -578,7 +639,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,12 +666,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="42"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -622,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -885,28 +940,6 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -1088,17 +1121,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -1160,49 +1182,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1248,22 +1233,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1274,10 +1250,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1285,10 +1261,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1296,22 +1272,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1329,36 +1305,32 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1370,6 +1342,21 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1381,30 +1368,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1816,10 +1785,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1837,662 +1806,711 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
+      <c r="F6" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="88"/>
+      <c r="C9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="88"/>
+      <c r="C10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="34"/>
+      <c r="H10" s="35"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="87" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="88"/>
+      <c r="C11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="87" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="88"/>
+      <c r="C12" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="1:10" ht="45" customHeight="1">
+      <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="10" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="90"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+    </row>
+    <row r="15" spans="1:10" s="32" customFormat="1">
+      <c r="A15" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="63"/>
+      <c r="C15" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="98" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="99"/>
-      <c r="C8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="98" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="98" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="99"/>
-      <c r="C10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="98" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="99"/>
-      <c r="C11" s="91" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:10" ht="45" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="100" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="101"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-    </row>
-    <row r="14" spans="1:10" s="32" customFormat="1">
-      <c r="A14" s="65" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14" s="69"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:10" s="32" customFormat="1">
-      <c r="A15" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67" t="s">
-        <v>17</v>
-      </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15" s="69"/>
+      <c r="G15" s="66"/>
       <c r="H15"/>
     </row>
     <row r="16" spans="1:10" s="32" customFormat="1">
-      <c r="A16" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="67"/>
+      <c r="A16" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="64" t="s">
+        <v>15</v>
+      </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="69"/>
+      <c r="G16" s="66"/>
       <c r="H16"/>
     </row>
     <row r="17" spans="1:12" s="32" customFormat="1">
-      <c r="A17" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67" t="s">
-        <v>17</v>
-      </c>
+      <c r="A17" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="69"/>
+      <c r="G17" s="66"/>
       <c r="H17"/>
     </row>
     <row r="18" spans="1:12" s="32" customFormat="1">
-      <c r="A18" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="67" t="s">
-        <v>17</v>
+      <c r="A18" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="63"/>
+      <c r="C18" s="64" t="s">
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="69"/>
+      <c r="G18" s="66"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:12" s="32" customFormat="1">
-      <c r="A19" s="92" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="93"/>
-      <c r="C19" s="67" t="s">
-        <v>17</v>
+      <c r="A19" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="64" t="s">
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="G19" s="69"/>
+      <c r="G19" s="66"/>
       <c r="H19"/>
     </row>
     <row r="20" spans="1:12" s="32" customFormat="1">
-      <c r="A20" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="67"/>
-      <c r="D20"/>
+      <c r="A20" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="93"/>
+      <c r="C20" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="G20" s="69"/>
+      <c r="G20" s="66"/>
       <c r="H20"/>
     </row>
     <row r="21" spans="1:12" s="32" customFormat="1">
-      <c r="A21" s="92" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>22</v>
-      </c>
+      <c r="A21" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="63"/>
+      <c r="C21" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="69"/>
+      <c r="G21" s="66"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:12" s="40" customFormat="1">
-      <c r="A22" s="37"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="47" t="s">
+    <row r="22" spans="1:12" s="32" customFormat="1">
+      <c r="A22" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="93"/>
+      <c r="C22" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22" s="66"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:12" s="37" customFormat="1">
+      <c r="A23" s="34"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="35"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="51"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="51"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="35"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="52"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="35"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="3" t="s">
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="103"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="38"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="37"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="30" t="s">
+      <c r="B31" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="35"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="51"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="35"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="51"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="35"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="52"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="35"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="83"/>
+      <c r="B35" s="84"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="35"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="15"/>
+    </row>
+    <row r="38" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A38" s="95" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="38"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="54"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="38"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="54"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="38"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="55"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="38"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="38"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="54"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="38"/>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="54"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="38"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="55"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="38"/>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="88"/>
-      <c r="B38" s="89"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="90"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="38"/>
+      <c r="G38" s="96" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="94"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="9"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
+      <c r="A39" s="95"/>
+      <c r="B39" s="95"/>
+      <c r="C39" s="94"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="97"/>
+      <c r="G39" s="97"/>
+      <c r="H39" s="94"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="15"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="6"/>
+      <c r="A40" s="19">
+        <v>1</v>
+      </c>
+      <c r="B40" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="69"/>
+      <c r="H40" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="28"/>
       <c r="L40" s="15"/>
     </row>
-    <row r="41" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A41" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="95" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="94" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="94" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="94" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="96" t="s">
-        <v>48</v>
-      </c>
-      <c r="G41" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" s="94" t="s">
+    <row r="41" spans="1:12">
+      <c r="A41" s="19">
+        <f>A40+1</f>
         <v>2</v>
       </c>
-      <c r="I41" s="94"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="17"/>
-      <c r="L41" s="9"/>
+      <c r="B41" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="20"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="15"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="95"/>
-      <c r="B42" s="95"/>
-      <c r="C42" s="94"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="94"/>
-      <c r="F42" s="97"/>
-      <c r="G42" s="97"/>
-      <c r="H42" s="94"/>
-      <c r="I42" s="94"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="29"/>
+      <c r="A42" s="19">
+        <f t="shared" ref="A42:A56" si="0">A41+1</f>
+        <v>3</v>
+      </c>
+      <c r="B42" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="22"/>
       <c r="L42" s="15"/>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="19">
-        <v>1</v>
-      </c>
-      <c r="B43" s="76"/>
-      <c r="C43" s="83"/>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B43" s="73" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="80" t="s">
+        <v>71</v>
+      </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="20"/>
+      <c r="G43" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="20" t="s">
+        <v>78</v>
+      </c>
       <c r="I43" s="21"/>
       <c r="J43" s="21"/>
-      <c r="K43" s="28"/>
+      <c r="K43" s="22"/>
       <c r="L43" s="15"/>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="19">
-        <f>A43+1</f>
-        <v>2</v>
-      </c>
-      <c r="B44" s="76"/>
-      <c r="C44" s="83"/>
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B44" s="73"/>
+      <c r="C44" s="80"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
-      <c r="G44" s="74"/>
+      <c r="G44" s="69"/>
       <c r="H44" s="20"/>
       <c r="I44" s="21"/>
       <c r="J44" s="21"/>
-      <c r="K44" s="28"/>
+      <c r="K44" s="22"/>
       <c r="L44" s="15"/>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="19">
-        <f t="shared" ref="A45:A59" si="0">A44+1</f>
-        <v>3</v>
-      </c>
-      <c r="B45" s="77"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="22"/>
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B45" s="73"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="75"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="77"/>
       <c r="L45" s="15"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="19">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B46" s="78"/>
-      <c r="C46" s="85"/>
+        <v>7</v>
+      </c>
+      <c r="B46" s="73"/>
+      <c r="C46" s="80"/>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
       <c r="F46" s="20"/>
-      <c r="G46" s="74"/>
+      <c r="G46" s="69"/>
       <c r="H46" s="20"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21"/>
@@ -2502,48 +2520,48 @@
     <row r="47" spans="1:12">
       <c r="A47" s="19">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B47" s="78"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="22"/>
+        <v>8</v>
+      </c>
+      <c r="B47" s="73"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="74"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="77"/>
       <c r="L47" s="15"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="19">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B48" s="78"/>
-      <c r="C48" s="85"/>
-      <c r="D48" s="79"/>
-      <c r="E48" s="79"/>
-      <c r="F48" s="79"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="81"/>
-      <c r="J48" s="81"/>
-      <c r="K48" s="82"/>
+        <v>9</v>
+      </c>
+      <c r="B48" s="73"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="76"/>
+      <c r="J48" s="76"/>
+      <c r="K48" s="77"/>
       <c r="L48" s="15"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="19">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B49" s="78"/>
-      <c r="C49" s="85"/>
+        <v>10</v>
+      </c>
+      <c r="B49" s="73"/>
+      <c r="C49" s="80"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
-      <c r="G49" s="74"/>
+      <c r="G49" s="69"/>
       <c r="H49" s="20"/>
       <c r="I49" s="21"/>
       <c r="J49" s="21"/>
@@ -2553,48 +2571,48 @@
     <row r="50" spans="1:12">
       <c r="A50" s="19">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B50" s="78"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="79"/>
-      <c r="F50" s="79"/>
-      <c r="G50" s="80"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="81"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="82"/>
+        <v>11</v>
+      </c>
+      <c r="B50" s="73"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="76"/>
+      <c r="J50" s="76"/>
+      <c r="K50" s="77"/>
       <c r="L50" s="15"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="19">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B51" s="78"/>
-      <c r="C51" s="85"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="79"/>
-      <c r="F51" s="79"/>
-      <c r="G51" s="80"/>
-      <c r="H51" s="79"/>
-      <c r="I51" s="81"/>
-      <c r="J51" s="81"/>
-      <c r="K51" s="82"/>
+        <v>12</v>
+      </c>
+      <c r="B51" s="73"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="75"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="76"/>
+      <c r="J51" s="76"/>
+      <c r="K51" s="77"/>
       <c r="L51" s="15"/>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="19">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B52" s="78"/>
-      <c r="C52" s="85"/>
+        <v>13</v>
+      </c>
+      <c r="B52" s="73"/>
+      <c r="C52" s="80"/>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
-      <c r="G52" s="74"/>
+      <c r="G52" s="69"/>
       <c r="H52" s="20"/>
       <c r="I52" s="21"/>
       <c r="J52" s="21"/>
@@ -2604,48 +2622,48 @@
     <row r="53" spans="1:12">
       <c r="A53" s="19">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B53" s="78"/>
-      <c r="C53" s="85"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="80"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="81"/>
-      <c r="J53" s="81"/>
-      <c r="K53" s="82"/>
+        <v>14</v>
+      </c>
+      <c r="B53" s="73"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="75"/>
+      <c r="H53" s="74"/>
+      <c r="I53" s="76"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="77"/>
       <c r="L53" s="15"/>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="19">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B54" s="78"/>
-      <c r="C54" s="85"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="79"/>
-      <c r="G54" s="80"/>
-      <c r="H54" s="79"/>
-      <c r="I54" s="81"/>
-      <c r="J54" s="81"/>
-      <c r="K54" s="82"/>
+        <v>15</v>
+      </c>
+      <c r="B54" s="73"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="75"/>
+      <c r="H54" s="74"/>
+      <c r="I54" s="76"/>
+      <c r="J54" s="76"/>
+      <c r="K54" s="77"/>
       <c r="L54" s="15"/>
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="19">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B55" s="78"/>
-      <c r="C55" s="85"/>
+        <v>16</v>
+      </c>
+      <c r="B55" s="73"/>
+      <c r="C55" s="80"/>
       <c r="D55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
-      <c r="G55" s="74"/>
+      <c r="G55" s="69"/>
       <c r="H55" s="20"/>
       <c r="I55" s="21"/>
       <c r="J55" s="21"/>
@@ -2655,122 +2673,68 @@
     <row r="56" spans="1:12">
       <c r="A56" s="19">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B56" s="78"/>
-      <c r="C56" s="85"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="79"/>
-      <c r="F56" s="79"/>
-      <c r="G56" s="80"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="81"/>
-      <c r="J56" s="81"/>
-      <c r="K56" s="82"/>
+        <v>17</v>
+      </c>
+      <c r="B56" s="73"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="74"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="76"/>
+      <c r="K56" s="77"/>
       <c r="L56" s="15"/>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="19">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B57" s="78"/>
-      <c r="C57" s="85"/>
-      <c r="D57" s="79"/>
-      <c r="E57" s="79"/>
-      <c r="F57" s="79"/>
-      <c r="G57" s="80"/>
-      <c r="H57" s="79"/>
-      <c r="I57" s="81"/>
-      <c r="J57" s="81"/>
-      <c r="K57" s="82"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="70"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="27"/>
       <c r="L57" s="15"/>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="A58" s="19">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B58" s="78"/>
-      <c r="C58" s="85"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="74"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="15"/>
-    </row>
-    <row r="59" spans="1:12">
-      <c r="A59" s="19">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B59" s="78"/>
-      <c r="C59" s="85"/>
-      <c r="D59" s="79"/>
-      <c r="E59" s="79"/>
-      <c r="F59" s="79"/>
-      <c r="G59" s="80"/>
-      <c r="H59" s="79"/>
-      <c r="I59" s="81"/>
-      <c r="J59" s="81"/>
-      <c r="K59" s="82"/>
-      <c r="L59" s="15"/>
-    </row>
-    <row r="60" spans="1:12">
-      <c r="A60" s="23"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="26"/>
-      <c r="J60" s="26"/>
-      <c r="K60" s="27"/>
-      <c r="L60" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H38:I39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H41:I42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E76:G76" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E73:G73" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:F60" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
-      <formula1>isAbstract</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C19 C15" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F40:G57 C16:C20" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
   </dataValidations>
@@ -2779,18 +2743,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;P / &amp;N ページ&amp;R&amp;D &amp;T</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4D7EF1AF-B173-884C-9E34-724A844BDD2E}">
-          <x14:formula1>
-            <xm:f>config!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>G43:G60</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2807,79 +2759,79 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="58" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="58" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="58" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="58" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="58" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="58" bestFit="1" customWidth="1"/>
-    <col min="11" max="251" width="8.83203125" style="58" customWidth="1"/>
-    <col min="252" max="16384" width="10.83203125" style="58"/>
+    <col min="1" max="3" width="8.83203125" style="55" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="55" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="55" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="55" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="55" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="11" max="251" width="8.83203125" style="55" customWidth="1"/>
+    <col min="252" max="16384" width="10.83203125" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="57" t="s">
+      <c r="H3" s="56" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="B3" s="59" t="s">
+      <c r="J3" s="56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="J4" s="58"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="59" t="s">
+      <c r="D5" s="60"/>
+      <c r="F5" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="B4" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="J4" s="61"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="63"/>
-      <c r="F5" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="63" t="s">
-        <v>16</v>
+      <c r="H5" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="60" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="64"/>
+      <c r="B6" s="61"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>

</xml_diff>

<commit_message>
Now we can generate component class! TODO: pages defitions for vue-router.
</commit_message>
<xml_diff>
--- a/meta/components/TableSample.xlsx
+++ b/meta/components/TableSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B50B1B-1803-E849-8D05-AC36CF7C7A84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0E7F67-6C16-F14C-BEB0-1E10941C0ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13200" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
   <si>
     <t>パッケージ</t>
   </si>
@@ -295,13 +295,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Vueコンポーネント定義・ヘッダ情報</t>
-    <rPh sb="0" eb="18">
-      <t xml:space="preserve">ジョウホウ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>/* import 文等、ファイル先頭に記述したいものはここに記載します。 */</t>
     <rPh sb="10" eb="11">
       <t xml:space="preserve">ブｎ </t>
@@ -585,6 +578,38 @@
     <t>四つ目のプロパティです</t>
     <rPh sb="0" eb="1">
       <t xml:space="preserve">４ツメ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>TitleHeader</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>BreadCrumbs</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { TitleHeader, BreadCrumbs } from "SampleComponents"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・ヘッダ情報（クラス用）</t>
+    <rPh sb="0" eb="18">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t xml:space="preserve">ヨウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・ヘッダ情報（インタフェイス用）</t>
+    <rPh sb="0" eb="18">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t xml:space="preserve">ヨウ </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1342,6 +1367,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1355,24 +1398,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1785,10 +1810,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1806,7 +1831,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -1839,19 +1864,19 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
       <c r="F6" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
@@ -1869,7 +1894,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="11"/>
@@ -1878,65 +1903,65 @@
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="88"/>
+      <c r="A9" s="93" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="94"/>
       <c r="C9" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="11"/>
       <c r="F9" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="87" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="88"/>
+      <c r="A10" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="94"/>
       <c r="C10" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
       <c r="F10" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="88"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
       <c r="F11" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="87" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="88"/>
+      <c r="A12" s="93" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="94"/>
       <c r="C12" s="86" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="11"/>
       <c r="F12" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="35"/>
@@ -1946,11 +1971,11 @@
         <v>1</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="89" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="90"/>
-      <c r="E13" s="91"/>
+      <c r="C13" s="95" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="96"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="65"/>
       <c r="G13" s="65"/>
       <c r="H13" s="34"/>
@@ -1991,14 +2016,14 @@
     </row>
     <row r="16" spans="1:10" s="32" customFormat="1">
       <c r="A16" s="62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="63"/>
       <c r="C16" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
@@ -2007,12 +2032,12 @@
     </row>
     <row r="17" spans="1:12" s="32" customFormat="1">
       <c r="A17" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="63"/>
       <c r="C17" s="64"/>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
@@ -2037,7 +2062,7 @@
     </row>
     <row r="19" spans="1:12" s="32" customFormat="1">
       <c r="A19" s="62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="63"/>
       <c r="C19" s="64" t="s">
@@ -2052,10 +2077,10 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:12" s="32" customFormat="1">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="93"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="64" t="s">
         <v>15</v>
       </c>
@@ -2082,10 +2107,10 @@
       <c r="H21"/>
     </row>
     <row r="22" spans="1:12" s="32" customFormat="1">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="93"/>
+      <c r="B22" s="88"/>
       <c r="C22" s="64" t="s">
         <v>15</v>
       </c>
@@ -2111,14 +2136,14 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="30" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
       <c r="E24" s="81"/>
       <c r="F24" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
@@ -2146,8 +2171,12 @@
       <c r="L25" s="35"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="51"/>
-      <c r="B26" s="46"/>
+      <c r="A26" s="51">
+        <v>1</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>80</v>
+      </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
       <c r="E26" s="39"/>
@@ -2200,14 +2229,14 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="30" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
       <c r="E30" s="81"/>
       <c r="F30" s="44" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
@@ -2221,7 +2250,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
@@ -2277,292 +2306,287 @@
       <c r="L34" s="35"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="83"/>
-      <c r="B35" s="84"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="35"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
+      <c r="A36" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="15"/>
-    </row>
-    <row r="38" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A38" s="95" t="s">
+      <c r="A37" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="95" t="s">
+      <c r="B37" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="35"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="51">
+        <v>1</v>
+      </c>
+      <c r="B38" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="35"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="51">
+        <v>2</v>
+      </c>
+      <c r="B39" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="35"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="52"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="35"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="83"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="35"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="15"/>
+    </row>
+    <row r="44" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A44" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="94" t="s">
+      <c r="C44" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="94" t="s">
+      <c r="D44" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="94" t="s">
+      <c r="E44" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="96" t="s">
-        <v>43</v>
-      </c>
-      <c r="G38" s="96" t="s">
+      <c r="F44" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="94" t="s">
+      <c r="H44" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="I38" s="94"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="9"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="95"/>
-      <c r="B39" s="95"/>
-      <c r="C39" s="94"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="97"/>
-      <c r="G39" s="97"/>
-      <c r="H39" s="94"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="15"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="19">
-        <v>1</v>
-      </c>
-      <c r="B40" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G40" s="69"/>
-      <c r="H40" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="15"/>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="19">
-        <f>A40+1</f>
-        <v>2</v>
-      </c>
-      <c r="B41" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="20"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="15"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="19">
-        <f t="shared" ref="A42:A56" si="0">A41+1</f>
-        <v>3</v>
-      </c>
-      <c r="B42" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="79" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="69" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="15"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B43" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="80" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="69" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="15"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="19">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B44" s="73"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="15"/>
+      <c r="I44" s="89"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="19">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B45" s="73"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="76"/>
-      <c r="J45" s="76"/>
-      <c r="K45" s="77"/>
+      <c r="A45" s="90"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="29"/>
       <c r="L45" s="15"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="19">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="80"/>
+        <v>1</v>
+      </c>
+      <c r="B46" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="78" t="s">
+        <v>63</v>
+      </c>
       <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
+      <c r="E46" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="G46" s="69"/>
-      <c r="H46" s="20"/>
+      <c r="H46" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="I46" s="21"/>
       <c r="J46" s="21"/>
-      <c r="K46" s="22"/>
+      <c r="K46" s="28"/>
       <c r="L46" s="15"/>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="19">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B47" s="73"/>
-      <c r="C47" s="80"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="74"/>
-      <c r="I47" s="76"/>
-      <c r="J47" s="76"/>
-      <c r="K47" s="77"/>
+        <f>A46+1</f>
+        <v>2</v>
+      </c>
+      <c r="B47" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="20"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="28"/>
       <c r="L47" s="15"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="19">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B48" s="73"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="75"/>
-      <c r="H48" s="74"/>
-      <c r="I48" s="76"/>
-      <c r="J48" s="76"/>
-      <c r="K48" s="77"/>
+        <f t="shared" ref="A48:A62" si="0">A47+1</f>
+        <v>3</v>
+      </c>
+      <c r="B48" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="22"/>
       <c r="L48" s="15"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="19">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B49" s="73"/>
-      <c r="C49" s="80"/>
+        <v>4</v>
+      </c>
+      <c r="B49" s="73" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="20"/>
+      <c r="G49" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="20" t="s">
+        <v>77</v>
+      </c>
       <c r="I49" s="21"/>
       <c r="J49" s="21"/>
       <c r="K49" s="22"/>
@@ -2571,24 +2595,24 @@
     <row r="50" spans="1:12">
       <c r="A50" s="19">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B50" s="73"/>
       <c r="C50" s="80"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="76"/>
-      <c r="J50" s="76"/>
-      <c r="K50" s="77"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="22"/>
       <c r="L50" s="15"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="19">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B51" s="73"/>
       <c r="C51" s="80"/>
@@ -2605,7 +2629,7 @@
     <row r="52" spans="1:12">
       <c r="A52" s="19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B52" s="73"/>
       <c r="C52" s="80"/>
@@ -2622,7 +2646,7 @@
     <row r="53" spans="1:12">
       <c r="A53" s="19">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B53" s="73"/>
       <c r="C53" s="80"/>
@@ -2639,7 +2663,7 @@
     <row r="54" spans="1:12">
       <c r="A54" s="19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B54" s="73"/>
       <c r="C54" s="80"/>
@@ -2656,7 +2680,7 @@
     <row r="55" spans="1:12">
       <c r="A55" s="19">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B55" s="73"/>
       <c r="C55" s="80"/>
@@ -2673,7 +2697,7 @@
     <row r="56" spans="1:12">
       <c r="A56" s="19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B56" s="73"/>
       <c r="C56" s="80"/>
@@ -2688,40 +2712,142 @@
       <c r="L56" s="15"/>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="23"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="70"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="27"/>
+      <c r="A57" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B57" s="73"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="74"/>
+      <c r="F57" s="74"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="74"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="77"/>
       <c r="L57" s="15"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="19">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B58" s="73"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="15"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="19">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B59" s="73"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="74"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="75"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="77"/>
+      <c r="L59" s="15"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B60" s="73"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="74"/>
+      <c r="E60" s="74"/>
+      <c r="F60" s="74"/>
+      <c r="G60" s="75"/>
+      <c r="H60" s="74"/>
+      <c r="I60" s="76"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="77"/>
+      <c r="L60" s="15"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="19">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B61" s="73"/>
+      <c r="C61" s="80"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="69"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="15"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B62" s="73"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="75"/>
+      <c r="H62" s="74"/>
+      <c r="I62" s="76"/>
+      <c r="J62" s="76"/>
+      <c r="K62" s="77"/>
+      <c r="L62" s="15"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="25"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="27"/>
+      <c r="L63" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H38:I39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="F38:F39"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H44:I45"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="F44:F45"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E73:G73" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E79:G79" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2731,7 +2857,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F40:G57 C16:C20" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F46:G63 C16:C20" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">

</xml_diff>

<commit_message>
0.0.8: Generate authRequired flag into meta of RouterConfig class.
</commit_message>
<xml_diff>
--- a/meta/components/TableSample.xlsx
+++ b/meta/components/TableSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0E7F67-6C16-F14C-BEB0-1E10941C0ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945CC591-66C6-BD45-B100-3794CD7B39DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="460" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -1367,6 +1367,21 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1383,21 +1398,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1813,7 +1813,7 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1903,10 +1903,10 @@
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="94"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="10" t="s">
         <v>50</v>
       </c>
@@ -1919,10 +1919,10 @@
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="94"/>
+      <c r="B10" s="88"/>
       <c r="C10" s="10" t="s">
         <v>54</v>
       </c>
@@ -1935,10 +1935,10 @@
       <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="94"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="10" t="s">
         <v>22</v>
       </c>
@@ -1951,10 +1951,10 @@
       <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="94"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="86" t="s">
         <v>61</v>
       </c>
@@ -1971,11 +1971,11 @@
         <v>1</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="91"/>
       <c r="F13" s="65"/>
       <c r="G13" s="65"/>
       <c r="H13" s="34"/>
@@ -2019,9 +2019,7 @@
         <v>47</v>
       </c>
       <c r="B16" s="63"/>
-      <c r="C16" s="64" t="s">
-        <v>15</v>
-      </c>
+      <c r="C16" s="64"/>
       <c r="D16" t="s">
         <v>46</v>
       </c>
@@ -2035,7 +2033,9 @@
         <v>48</v>
       </c>
       <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
+      <c r="C17" s="64" t="s">
+        <v>15</v>
+      </c>
       <c r="D17" t="s">
         <v>46</v>
       </c>
@@ -2077,10 +2077,10 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:12" s="32" customFormat="1">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="88"/>
+      <c r="B20" s="93"/>
       <c r="C20" s="64" t="s">
         <v>15</v>
       </c>
@@ -2107,10 +2107,10 @@
       <c r="H21"/>
     </row>
     <row r="22" spans="1:12" s="32" customFormat="1">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="88"/>
+      <c r="B22" s="93"/>
       <c r="C22" s="64" t="s">
         <v>15</v>
       </c>
@@ -2446,45 +2446,45 @@
       <c r="L43" s="15"/>
     </row>
     <row r="44" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="90" t="s">
+      <c r="B44" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="89" t="s">
+      <c r="C44" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="89" t="s">
+      <c r="D44" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="89" t="s">
+      <c r="E44" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="91" t="s">
+      <c r="F44" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G44" s="91" t="s">
+      <c r="G44" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="89" t="s">
+      <c r="H44" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="89"/>
+      <c r="I44" s="94"/>
       <c r="J44" s="16"/>
       <c r="K44" s="17"/>
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="90"/>
-      <c r="B45" s="90"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
+      <c r="A45" s="95"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="94"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="94"/>
       <c r="J45" s="18"/>
       <c r="K45" s="29"/>
       <c r="L45" s="15"/>
@@ -2829,11 +2829,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:E13"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H44:I45"/>
@@ -2844,6 +2839,11 @@
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="G44:G45"/>
     <mergeCell ref="F44:F45"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">

</xml_diff>

<commit_message>
0.0.9: Enable GET query string parameters mapping to props. Generate Prop for componentId.
</commit_message>
<xml_diff>
--- a/meta/components/TableSample.xlsx
+++ b/meta/components/TableSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945CC591-66C6-BD45-B100-3794CD7B39DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BD062F-20E8-5847-9253-2C66F91D0760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="460" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
   <si>
     <t>パッケージ</t>
   </si>
@@ -610,6 +610,40 @@
     </rPh>
     <rPh sb="26" eb="27">
       <t xml:space="preserve">ヨウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>クエリ文字列</t>
+    <rPh sb="3" eb="6">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prop05</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>first</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>クエリ文字列パラメータのテストです。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>prop06</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>second</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>クエリ文字列パラメータのテストです。</t>
+    <rPh sb="0" eb="3">
+      <t>クエリ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1212,7 +1246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1392,6 +1426,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1810,10 +1850,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1821,33 +1861,33 @@
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="5" width="23.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28" style="1" customWidth="1"/>
-    <col min="11" max="11" width="33.33203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="7" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19">
+    <row r="1" spans="1:11" ht="19">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1857,8 +1897,9 @@
       <c r="E5" s="5"/>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1872,9 +1913,10 @@
         <v>75</v>
       </c>
       <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
@@ -1886,9 +1928,10 @@
       <c r="E7" s="8"/>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1900,9 +1943,10 @@
       <c r="E8" s="11"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="H8" s="34"/>
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="87" t="s">
         <v>57</v>
       </c>
@@ -1916,9 +1960,10 @@
         <v>51</v>
       </c>
       <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="87" t="s">
         <v>58</v>
       </c>
@@ -1932,9 +1977,10 @@
         <v>55</v>
       </c>
       <c r="G10" s="34"/>
-      <c r="H10" s="35"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="87" t="s">
         <v>21</v>
       </c>
@@ -1948,9 +1994,10 @@
         <v>52</v>
       </c>
       <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="H11" s="34"/>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="87" t="s">
         <v>49</v>
       </c>
@@ -1964,9 +2011,10 @@
         <v>53</v>
       </c>
       <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="1:10" ht="45" customHeight="1">
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+    </row>
+    <row r="13" spans="1:11" ht="45" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1978,11 +2026,12 @@
       <c r="E13" s="91"/>
       <c r="F13" s="65"/>
       <c r="G13" s="65"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="65"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="34"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1997,8 +2046,9 @@
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
-    </row>
-    <row r="15" spans="1:10" s="32" customFormat="1">
+      <c r="K14" s="34"/>
+    </row>
+    <row r="15" spans="1:11" s="32" customFormat="1">
       <c r="A15" s="62" t="s">
         <v>29</v>
       </c>
@@ -2012,9 +2062,10 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" s="66"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:10" s="32" customFormat="1">
+      <c r="H15" s="66"/>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:11" s="32" customFormat="1">
       <c r="A16" s="62" t="s">
         <v>47</v>
       </c>
@@ -2026,9 +2077,10 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" s="66"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:12" s="32" customFormat="1">
+      <c r="H16" s="66"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="1:13" s="32" customFormat="1">
       <c r="A17" s="62" t="s">
         <v>48</v>
       </c>
@@ -2042,9 +2094,10 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" s="66"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:12" s="32" customFormat="1">
+      <c r="H17" s="66"/>
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="1:13" s="32" customFormat="1">
       <c r="A18" s="62" t="s">
         <v>34</v>
       </c>
@@ -2058,9 +2111,10 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" s="66"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:12" s="32" customFormat="1">
+      <c r="H18" s="66"/>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:13" s="32" customFormat="1">
       <c r="A19" s="62" t="s">
         <v>59</v>
       </c>
@@ -2074,9 +2128,10 @@
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19" s="66"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:12" s="32" customFormat="1">
+      <c r="H19" s="66"/>
+      <c r="I19"/>
+    </row>
+    <row r="20" spans="1:13" s="32" customFormat="1">
       <c r="A20" s="92" t="s">
         <v>33</v>
       </c>
@@ -2090,9 +2145,10 @@
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20" s="66"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:12" s="32" customFormat="1">
+      <c r="H20" s="66"/>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:13" s="32" customFormat="1">
       <c r="A21" s="62" t="s">
         <v>16</v>
       </c>
@@ -2104,9 +2160,10 @@
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21" s="66"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:12" s="32" customFormat="1">
+      <c r="H21" s="66"/>
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:13" s="32" customFormat="1">
       <c r="A22" s="92" t="s">
         <v>19</v>
       </c>
@@ -2120,9 +2177,10 @@
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22" s="66"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:12" s="37" customFormat="1">
+      <c r="H22" s="66"/>
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:13" s="37" customFormat="1">
       <c r="A23" s="34"/>
       <c r="B23" s="36"/>
       <c r="C23" s="34"/>
@@ -2133,8 +2191,9 @@
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
       <c r="J23" s="34"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="K23" s="34"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="30" t="s">
         <v>81</v>
       </c>
@@ -2147,12 +2206,13 @@
       </c>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
-      <c r="I24" s="43"/>
+      <c r="I24" s="44"/>
       <c r="J24" s="43"/>
       <c r="K24" s="43"/>
       <c r="L24" s="43"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="43"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="47" t="s">
         <v>8</v>
       </c>
@@ -2165,12 +2225,13 @@
       <c r="F25" s="67"/>
       <c r="G25" s="67"/>
       <c r="H25" s="67"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="45"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="44"/>
       <c r="K25" s="45"/>
-      <c r="L25" s="35"/>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="L25" s="45"/>
+      <c r="M25" s="35"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="51">
         <v>1</v>
       </c>
@@ -2182,13 +2243,14 @@
       <c r="E26" s="39"/>
       <c r="F26" s="68"/>
       <c r="G26" s="68"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="36"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="34"/>
       <c r="J26" s="36"/>
       <c r="K26" s="36"/>
-      <c r="L26" s="35"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="L26" s="36"/>
+      <c r="M26" s="35"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="51"/>
       <c r="B27" s="46"/>
       <c r="C27" s="40"/>
@@ -2196,13 +2258,14 @@
       <c r="E27" s="41"/>
       <c r="F27" s="68"/>
       <c r="G27" s="68"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="36"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="34"/>
       <c r="J27" s="36"/>
       <c r="K27" s="36"/>
-      <c r="L27" s="35"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="L27" s="36"/>
+      <c r="M27" s="35"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="52"/>
       <c r="B28" s="48"/>
       <c r="C28" s="49"/>
@@ -2210,13 +2273,14 @@
       <c r="E28" s="50"/>
       <c r="F28" s="68"/>
       <c r="G28" s="68"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="36"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="34"/>
       <c r="J28" s="36"/>
       <c r="K28" s="36"/>
-      <c r="L28" s="35"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="L28" s="36"/>
+      <c r="M28" s="35"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -2226,8 +2290,9 @@
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="30" t="s">
         <v>82</v>
       </c>
@@ -2240,12 +2305,13 @@
       </c>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
-      <c r="I30" s="43"/>
+      <c r="I30" s="44"/>
       <c r="J30" s="43"/>
       <c r="K30" s="43"/>
       <c r="L30" s="43"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" s="43"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="47" t="s">
         <v>8</v>
       </c>
@@ -2258,12 +2324,13 @@
       <c r="F31" s="67"/>
       <c r="G31" s="67"/>
       <c r="H31" s="67"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="45"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="44"/>
       <c r="K31" s="45"/>
-      <c r="L31" s="35"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="L31" s="45"/>
+      <c r="M31" s="35"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="51"/>
       <c r="B32" s="46"/>
       <c r="C32" s="38"/>
@@ -2271,13 +2338,14 @@
       <c r="E32" s="39"/>
       <c r="F32" s="68"/>
       <c r="G32" s="68"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="36"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="34"/>
       <c r="J32" s="36"/>
       <c r="K32" s="36"/>
-      <c r="L32" s="35"/>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="L32" s="36"/>
+      <c r="M32" s="35"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="51"/>
       <c r="B33" s="46"/>
       <c r="C33" s="40"/>
@@ -2285,13 +2353,14 @@
       <c r="E33" s="41"/>
       <c r="F33" s="68"/>
       <c r="G33" s="68"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="36"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="34"/>
       <c r="J33" s="36"/>
       <c r="K33" s="36"/>
-      <c r="L33" s="35"/>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="L33" s="36"/>
+      <c r="M33" s="35"/>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="52"/>
       <c r="B34" s="48"/>
       <c r="C34" s="49"/>
@@ -2299,13 +2368,14 @@
       <c r="E34" s="50"/>
       <c r="F34" s="68"/>
       <c r="G34" s="68"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="36"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="34"/>
       <c r="J34" s="36"/>
       <c r="K34" s="36"/>
-      <c r="L34" s="35"/>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="L34" s="36"/>
+      <c r="M34" s="35"/>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -2315,8 +2385,9 @@
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="30" t="s">
         <v>43</v>
       </c>
@@ -2329,12 +2400,13 @@
       </c>
       <c r="G36" s="44"/>
       <c r="H36" s="44"/>
-      <c r="I36" s="43"/>
+      <c r="I36" s="44"/>
       <c r="J36" s="43"/>
       <c r="K36" s="43"/>
       <c r="L36" s="43"/>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" s="43"/>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="47" t="s">
         <v>8</v>
       </c>
@@ -2347,12 +2419,13 @@
       <c r="F37" s="67"/>
       <c r="G37" s="67"/>
       <c r="H37" s="67"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="45"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="44"/>
       <c r="K37" s="45"/>
-      <c r="L37" s="35"/>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="L37" s="45"/>
+      <c r="M37" s="35"/>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="51">
         <v>1</v>
       </c>
@@ -2364,13 +2437,14 @@
       <c r="E38" s="39"/>
       <c r="F38" s="68"/>
       <c r="G38" s="68"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="36"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="34"/>
       <c r="J38" s="36"/>
       <c r="K38" s="36"/>
-      <c r="L38" s="35"/>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="L38" s="36"/>
+      <c r="M38" s="35"/>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="51">
         <v>2</v>
       </c>
@@ -2382,13 +2456,14 @@
       <c r="E39" s="41"/>
       <c r="F39" s="68"/>
       <c r="G39" s="68"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="36"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="34"/>
       <c r="J39" s="36"/>
       <c r="K39" s="36"/>
-      <c r="L39" s="35"/>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="L39" s="36"/>
+      <c r="M39" s="35"/>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="52"/>
       <c r="B40" s="48"/>
       <c r="C40" s="49"/>
@@ -2396,13 +2471,14 @@
       <c r="E40" s="50"/>
       <c r="F40" s="68"/>
       <c r="G40" s="68"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="36"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="34"/>
       <c r="J40" s="36"/>
       <c r="K40" s="36"/>
-      <c r="L40" s="35"/>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="L40" s="36"/>
+      <c r="M40" s="35"/>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="83"/>
       <c r="B41" s="84"/>
       <c r="C41" s="85"/>
@@ -2410,13 +2486,14 @@
       <c r="E41" s="85"/>
       <c r="F41" s="68"/>
       <c r="G41" s="68"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="36"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="34"/>
       <c r="J41" s="36"/>
       <c r="K41" s="36"/>
-      <c r="L41" s="35"/>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="L41" s="36"/>
+      <c r="M41" s="35"/>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="13"/>
       <c r="B42" s="13" t="s">
         <v>45</v>
@@ -2428,8 +2505,9 @@
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="J42" s="13"/>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="3" t="s">
         <v>40</v>
       </c>
@@ -2442,10 +2520,11 @@
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="15"/>
-    </row>
-    <row r="44" spans="1:12" ht="13.5" customHeight="1">
+      <c r="K43" s="14"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="15"/>
+    </row>
+    <row r="44" spans="1:13" ht="13.5" customHeight="1">
       <c r="A44" s="95" t="s">
         <v>8</v>
       </c>
@@ -2461,35 +2540,39 @@
       <c r="E44" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="96" t="s">
+      <c r="F44" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="G44" s="96" t="s">
+      <c r="G44" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="94" t="s">
+      <c r="H44" s="96" t="s">
+        <v>83</v>
+      </c>
+      <c r="I44" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="94"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="9"/>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="J44" s="94"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="9"/>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="95"/>
       <c r="B45" s="95"/>
       <c r="C45" s="94"/>
       <c r="D45" s="94"/>
       <c r="E45" s="94"/>
-      <c r="F45" s="97"/>
-      <c r="G45" s="97"/>
-      <c r="H45" s="94"/>
+      <c r="F45" s="99"/>
+      <c r="G45" s="99"/>
+      <c r="H45" s="97"/>
       <c r="I45" s="94"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="15"/>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="J45" s="94"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="15"/>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="19">
         <v>1</v>
       </c>
@@ -2507,15 +2590,16 @@
         <v>15</v>
       </c>
       <c r="G46" s="69"/>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="69"/>
+      <c r="I46" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="I46" s="21"/>
       <c r="J46" s="21"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="15"/>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="K46" s="21"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="15"/>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="19">
         <f>A46+1</f>
         <v>2</v>
@@ -2532,15 +2616,16 @@
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="69"/>
-      <c r="H47" s="20" t="s">
+      <c r="H47" s="69"/>
+      <c r="I47" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="I47" s="21"/>
       <c r="J47" s="21"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="15"/>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="K47" s="21"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="15"/>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="19">
         <f t="shared" ref="A48:A62" si="0">A47+1</f>
         <v>3</v>
@@ -2559,15 +2644,16 @@
       <c r="G48" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="20" t="s">
+      <c r="H48" s="69"/>
+      <c r="I48" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="I48" s="21"/>
       <c r="J48" s="21"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="15"/>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="K48" s="21"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="15"/>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2584,49 +2670,72 @@
       <c r="G49" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="H49" s="20" t="s">
+      <c r="H49" s="69"/>
+      <c r="I49" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="I49" s="21"/>
       <c r="J49" s="21"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="15"/>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="K49" s="21"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="15"/>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B50" s="73"/>
-      <c r="C50" s="80"/>
+      <c r="B50" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="80" t="s">
+        <v>63</v>
+      </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="21"/>
+      <c r="G50" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="I50" s="20" t="s">
+        <v>86</v>
+      </c>
       <c r="J50" s="21"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="15"/>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="K50" s="21"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="15"/>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B51" s="73"/>
-      <c r="C51" s="80"/>
+      <c r="B51" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="80" t="s">
+        <v>63</v>
+      </c>
       <c r="D51" s="74"/>
       <c r="E51" s="74"/>
       <c r="F51" s="74"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="74"/>
-      <c r="I51" s="76"/>
+      <c r="G51" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="I51" s="74" t="s">
+        <v>89</v>
+      </c>
       <c r="J51" s="76"/>
-      <c r="K51" s="77"/>
-      <c r="L51" s="15"/>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="K51" s="76"/>
+      <c r="L51" s="77"/>
+      <c r="M51" s="15"/>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="19">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2637,13 +2746,14 @@
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
       <c r="G52" s="69"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="21"/>
+      <c r="H52" s="69"/>
+      <c r="I52" s="20"/>
       <c r="J52" s="21"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="15"/>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="K52" s="21"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="15"/>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2654,13 +2764,14 @@
       <c r="E53" s="74"/>
       <c r="F53" s="74"/>
       <c r="G53" s="75"/>
-      <c r="H53" s="74"/>
-      <c r="I53" s="76"/>
+      <c r="H53" s="75"/>
+      <c r="I53" s="74"/>
       <c r="J53" s="76"/>
-      <c r="K53" s="77"/>
-      <c r="L53" s="15"/>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="K53" s="76"/>
+      <c r="L53" s="77"/>
+      <c r="M53" s="15"/>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2671,13 +2782,14 @@
       <c r="E54" s="74"/>
       <c r="F54" s="74"/>
       <c r="G54" s="75"/>
-      <c r="H54" s="74"/>
-      <c r="I54" s="76"/>
+      <c r="H54" s="75"/>
+      <c r="I54" s="74"/>
       <c r="J54" s="76"/>
-      <c r="K54" s="77"/>
-      <c r="L54" s="15"/>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="K54" s="76"/>
+      <c r="L54" s="77"/>
+      <c r="M54" s="15"/>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2688,13 +2800,14 @@
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
       <c r="G55" s="69"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="21"/>
+      <c r="H55" s="69"/>
+      <c r="I55" s="20"/>
       <c r="J55" s="21"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="15"/>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="K55" s="21"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="15"/>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2705,13 +2818,14 @@
       <c r="E56" s="74"/>
       <c r="F56" s="74"/>
       <c r="G56" s="75"/>
-      <c r="H56" s="74"/>
-      <c r="I56" s="76"/>
+      <c r="H56" s="75"/>
+      <c r="I56" s="74"/>
       <c r="J56" s="76"/>
-      <c r="K56" s="77"/>
-      <c r="L56" s="15"/>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="K56" s="76"/>
+      <c r="L56" s="77"/>
+      <c r="M56" s="15"/>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="19">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2722,13 +2836,14 @@
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
       <c r="G57" s="75"/>
-      <c r="H57" s="74"/>
-      <c r="I57" s="76"/>
+      <c r="H57" s="75"/>
+      <c r="I57" s="74"/>
       <c r="J57" s="76"/>
-      <c r="K57" s="77"/>
-      <c r="L57" s="15"/>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="K57" s="76"/>
+      <c r="L57" s="77"/>
+      <c r="M57" s="15"/>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="19">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2739,13 +2854,14 @@
       <c r="E58" s="20"/>
       <c r="F58" s="20"/>
       <c r="G58" s="69"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="21"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="20"/>
       <c r="J58" s="21"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="15"/>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="K58" s="21"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="15"/>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="19">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2756,13 +2872,14 @@
       <c r="E59" s="74"/>
       <c r="F59" s="74"/>
       <c r="G59" s="75"/>
-      <c r="H59" s="74"/>
-      <c r="I59" s="76"/>
+      <c r="H59" s="75"/>
+      <c r="I59" s="74"/>
       <c r="J59" s="76"/>
-      <c r="K59" s="77"/>
-      <c r="L59" s="15"/>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="K59" s="76"/>
+      <c r="L59" s="77"/>
+      <c r="M59" s="15"/>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="19">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2773,13 +2890,14 @@
       <c r="E60" s="74"/>
       <c r="F60" s="74"/>
       <c r="G60" s="75"/>
-      <c r="H60" s="74"/>
-      <c r="I60" s="76"/>
+      <c r="H60" s="75"/>
+      <c r="I60" s="74"/>
       <c r="J60" s="76"/>
-      <c r="K60" s="77"/>
-      <c r="L60" s="15"/>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="K60" s="76"/>
+      <c r="L60" s="77"/>
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2790,13 +2908,14 @@
       <c r="E61" s="20"/>
       <c r="F61" s="20"/>
       <c r="G61" s="69"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="21"/>
+      <c r="H61" s="69"/>
+      <c r="I61" s="20"/>
       <c r="J61" s="21"/>
-      <c r="K61" s="22"/>
-      <c r="L61" s="15"/>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="K61" s="21"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="15"/>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2807,13 +2926,14 @@
       <c r="E62" s="74"/>
       <c r="F62" s="74"/>
       <c r="G62" s="75"/>
-      <c r="H62" s="74"/>
-      <c r="I62" s="76"/>
+      <c r="H62" s="75"/>
+      <c r="I62" s="74"/>
       <c r="J62" s="76"/>
-      <c r="K62" s="77"/>
-      <c r="L62" s="15"/>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="K62" s="76"/>
+      <c r="L62" s="77"/>
+      <c r="M62" s="15"/>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="23"/>
       <c r="B63" s="24"/>
       <c r="C63" s="25"/>
@@ -2821,24 +2941,26 @@
       <c r="E63" s="25"/>
       <c r="F63" s="25"/>
       <c r="G63" s="70"/>
-      <c r="H63" s="25"/>
-      <c r="I63" s="26"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="25"/>
       <c r="J63" s="26"/>
-      <c r="K63" s="27"/>
-      <c r="L63" s="15"/>
+      <c r="K63" s="26"/>
+      <c r="L63" s="27"/>
+      <c r="M63" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H44:I45"/>
+    <mergeCell ref="I44:J45"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="E44:E45"/>
     <mergeCell ref="D44:D45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="F44:F45"/>
     <mergeCell ref="G44:G45"/>
-    <mergeCell ref="F44:F45"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
@@ -2847,7 +2969,7 @@
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E79:G79" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E79:H79" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2857,7 +2979,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F46:G63 C16:C20" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C20 F46:G63" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">

</xml_diff>